<commit_message>
updated the project management doc
IOS developer account
</commit_message>
<xml_diff>
--- a/项目管理.xlsx
+++ b/项目管理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="约定" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="125">
   <si>
     <t>产生日期</t>
   </si>
@@ -396,6 +396,9 @@
   </si>
   <si>
     <t>F-IL-INDOOFLOCATION-ST</t>
+  </si>
+  <si>
+    <t>ios develop account</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="yyyy/m/d;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/m/d;@"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -639,26 +642,26 @@
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="14" fontId="8" fillId="3" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1042,9 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1078,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1108,6 +1109,11 @@
       </c>
       <c r="E1" s="13" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="C2" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1881,7 +1887,7 @@
       <c r="D1" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="22" t="s">
         <v>79</v>
       </c>
     </row>
@@ -2352,103 +2358,103 @@
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="24" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="25">
         <v>41881</v>
       </c>
       <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="18"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C3" s="21"/>
+      <c r="C3" s="25"/>
       <c r="E3" s="10"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="18"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="21"/>
+      <c r="C4" s="25"/>
       <c r="E4" s="10"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="18"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C5" s="21"/>
+      <c r="C5" s="25"/>
       <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="18"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C6" s="21"/>
+      <c r="C6" s="25"/>
       <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="18"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="25"/>
       <c r="E7" s="10"/>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="18"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="21"/>
+      <c r="C8" s="25"/>
       <c r="E8" s="10"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="18"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="21"/>
+      <c r="C9" s="25"/>
       <c r="E9" s="10"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="18"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="C10" s="21"/>
+      <c r="C10" s="25"/>
       <c r="E10" s="10"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="18"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C11" s="21"/>
+      <c r="C11" s="25"/>
       <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="18"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="21"/>
+      <c r="C12" s="25"/>
       <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="22">
+      <c r="B13" s="18"/>
+      <c r="C13" s="20">
         <f>SUM(C2+15)</f>
         <v>41896</v>
       </c>
@@ -2457,8 +2463,8 @@
       <c r="A14" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="23">
+      <c r="B14" s="19"/>
+      <c r="C14" s="21">
         <f t="shared" ref="C14:C16" si="0">SUM(C13+15)</f>
         <v>41911</v>
       </c>
@@ -2467,8 +2473,8 @@
       <c r="A15" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="22">
+      <c r="B15" s="18"/>
+      <c r="C15" s="20">
         <f>SUM(C14+19)</f>
         <v>41930</v>
       </c>
@@ -2477,8 +2483,8 @@
       <c r="A16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="23">
+      <c r="B16" s="19"/>
+      <c r="C16" s="21">
         <f t="shared" si="0"/>
         <v>41945</v>
       </c>
@@ -2502,7 +2508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2525,7 +2531,7 @@
       <c r="C1" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="25"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="2" t="s">
         <v>90</v>
       </c>
@@ -2560,7 +2566,7 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="24" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2571,7 +2577,7 @@
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="18"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
         <v>110</v>
       </c>
@@ -2580,7 +2586,7 @@
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="18"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
         <v>111</v>
       </c>
@@ -2589,7 +2595,7 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="18"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
         <v>120</v>
       </c>
@@ -2598,7 +2604,7 @@
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="18"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
         <v>112</v>
       </c>
@@ -2607,7 +2613,7 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="18"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
         <v>113</v>
       </c>
@@ -2616,7 +2622,7 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="18"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
         <v>114</v>
       </c>
@@ -2625,7 +2631,7 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="18"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
         <v>115</v>
       </c>
@@ -2634,14 +2640,14 @@
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="18"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="4" t="s">
         <v>121</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="18"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="4" t="s">
         <v>122</v>
       </c>
@@ -2650,7 +2656,7 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="18"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="4" t="s">
         <v>123</v>
       </c>
@@ -2659,7 +2665,7 @@
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="18"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="4" t="s">
         <v>96</v>
       </c>
@@ -2668,7 +2674,7 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="18"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="4" t="s">
         <v>85</v>
       </c>

</xml_diff>

<commit_message>
Updated the name of 沈哥
</commit_message>
<xml_diff>
--- a/项目管理.xlsx
+++ b/项目管理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="约定" sheetId="1" r:id="rId1"/>
@@ -317,9 +317,6 @@
     <t>Review</t>
   </si>
   <si>
-    <t>沈议、徐实</t>
-  </si>
-  <si>
     <t>附近商铺信息维护</t>
   </si>
   <si>
@@ -399,6 +396,9 @@
   </si>
   <si>
     <t>ios develop account</t>
+  </si>
+  <si>
+    <t>沈毅、徐实</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="C2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1252,7 +1252,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>32</v>
@@ -1954,7 +1954,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>65</v>
@@ -1967,7 +1967,7 @@
     <row r="7" spans="1:5">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>59</v>
@@ -1980,7 +1980,7 @@
     <row r="8" spans="1:5">
       <c r="A8" s="4"/>
       <c r="B8" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>60</v>
@@ -1993,7 +1993,7 @@
     <row r="9" spans="1:5">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>61</v>
@@ -2006,7 +2006,7 @@
     <row r="10" spans="1:5">
       <c r="A10" s="4"/>
       <c r="B10" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>70</v>
@@ -2017,7 +2017,7 @@
     <row r="11" spans="1:5">
       <c r="A11" s="4"/>
       <c r="B11" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>71</v>
@@ -2084,7 +2084,7 @@
         <v>39</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>72</v>
@@ -2097,7 +2097,7 @@
     <row r="19" spans="1:5">
       <c r="A19" s="1"/>
       <c r="B19" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>73</v>
@@ -2112,7 +2112,7 @@
     <row r="20" spans="1:5">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>76</v>
@@ -2125,7 +2125,7 @@
     <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>70</v>
@@ -2362,7 +2362,7 @@
         <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="25">
         <v>41881</v>
@@ -2372,7 +2372,7 @@
     <row r="3" spans="1:10">
       <c r="A3" s="24"/>
       <c r="B3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="25"/>
       <c r="E3" s="10"/>
@@ -2380,7 +2380,7 @@
     <row r="4" spans="1:10">
       <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C4" s="25"/>
       <c r="E4" s="10"/>
@@ -2388,7 +2388,7 @@
     <row r="5" spans="1:10">
       <c r="A5" s="24"/>
       <c r="B5" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C5" s="25"/>
       <c r="E5" s="10"/>
@@ -2396,7 +2396,7 @@
     <row r="6" spans="1:10">
       <c r="A6" s="24"/>
       <c r="B6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C6" s="25"/>
       <c r="E6" s="10"/>
@@ -2404,7 +2404,7 @@
     <row r="7" spans="1:10">
       <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C7" s="25"/>
       <c r="E7" s="10"/>
@@ -2412,7 +2412,7 @@
     <row r="8" spans="1:10">
       <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="25"/>
       <c r="E8" s="10"/>
@@ -2420,7 +2420,7 @@
     <row r="9" spans="1:10">
       <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="25"/>
       <c r="E9" s="10"/>
@@ -2428,7 +2428,7 @@
     <row r="10" spans="1:10">
       <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C10" s="25"/>
       <c r="E10" s="10"/>
@@ -2436,7 +2436,7 @@
     <row r="11" spans="1:10">
       <c r="A11" s="24"/>
       <c r="B11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C11" s="25"/>
       <c r="E11" s="10"/>
@@ -2444,7 +2444,7 @@
     <row r="12" spans="1:10">
       <c r="A12" s="24"/>
       <c r="B12" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C12" s="25"/>
       <c r="E12" s="10"/>
@@ -2508,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2570,7 +2570,7 @@
         <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>92</v>
@@ -2579,7 +2579,7 @@
     <row r="4" spans="1:8">
       <c r="A4" s="24"/>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>92</v>
@@ -2588,7 +2588,7 @@
     <row r="5" spans="1:8">
       <c r="A5" s="24"/>
       <c r="B5" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>92</v>
@@ -2597,7 +2597,7 @@
     <row r="6" spans="1:8">
       <c r="A6" s="24"/>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>93</v>
@@ -2606,7 +2606,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="24"/>
       <c r="B7" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>93</v>
@@ -2615,7 +2615,7 @@
     <row r="8" spans="1:8">
       <c r="A8" s="24"/>
       <c r="B8" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>93</v>
@@ -2624,16 +2624,16 @@
     <row r="9" spans="1:8">
       <c r="A9" s="24"/>
       <c r="B9" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="24"/>
       <c r="B10" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>93</v>
@@ -2642,14 +2642,14 @@
     <row r="11" spans="1:8">
       <c r="A11" s="24"/>
       <c r="B11" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="24"/>
       <c r="B12" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G12" t="s">
         <v>94</v>
@@ -2658,7 +2658,7 @@
     <row r="13" spans="1:8">
       <c r="A13" s="24"/>
       <c r="B13" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G13" t="s">
         <v>94</v>

</xml_diff>